<commit_message>
a small fix in expense in anjum saeed expence
</commit_message>
<xml_diff>
--- a/Expenditures/Expenditure Mian Anjum Saeed.xlsx
+++ b/Expenditures/Expenditure Mian Anjum Saeed.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Z\Documents\Mian-Industries\Expenditures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7D4FB2E-220C-4CDD-A950-BBAA44776962}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5BECAC5-F50B-4A68-B46B-00129B8E4BF1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="43">
   <si>
     <t>Date</t>
   </si>
@@ -154,21 +154,6 @@
   </si>
   <si>
     <t>Advance from pay</t>
-  </si>
-  <si>
-    <t>Ali</t>
-  </si>
-  <si>
-    <t>Cement for roof</t>
-  </si>
-  <si>
-    <t>Dahari mistri</t>
-  </si>
-  <si>
-    <t>Basit</t>
-  </si>
-  <si>
-    <t>Lunch for arshad sb</t>
   </si>
 </sst>
 </file>
@@ -774,7 +759,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="A33" sqref="A33:D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -812,7 +797,7 @@
       <c r="J1" s="28"/>
       <c r="K1" s="6">
         <f>D93</f>
-        <v>215714</v>
+        <v>202714</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="14.25" customHeight="1">
@@ -830,7 +815,7 @@
       <c r="J2" s="31"/>
       <c r="K2" s="10">
         <f>F95</f>
-        <v>34286</v>
+        <v>47286</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="14.25" customHeight="1">
@@ -1404,60 +1389,36 @@
       </c>
     </row>
     <row r="33" spans="1:6" ht="14.25" customHeight="1">
-      <c r="A33" s="16">
-        <v>45859</v>
-      </c>
-      <c r="B33" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="C33" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="D33" s="13">
-        <v>6750</v>
-      </c>
+      <c r="A33" s="16"/>
+      <c r="B33" s="15"/>
+      <c r="C33" s="15"/>
+      <c r="D33" s="13"/>
       <c r="E33" s="14"/>
       <c r="F33" s="9">
         <f t="shared" si="0"/>
-        <v>40536</v>
+        <v>47286</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="14.25" customHeight="1">
-      <c r="A34" s="17">
-        <v>45859</v>
-      </c>
-      <c r="B34" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="C34" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="D34" s="13">
-        <v>4500</v>
-      </c>
+      <c r="A34" s="17"/>
+      <c r="B34" s="15"/>
+      <c r="C34" s="15"/>
+      <c r="D34" s="13"/>
       <c r="E34" s="14"/>
       <c r="F34" s="9">
         <f t="shared" si="0"/>
-        <v>36036</v>
+        <v>47286</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="14.25" customHeight="1">
-      <c r="A35" s="17">
-        <v>45859</v>
-      </c>
-      <c r="B35" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="C35" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="D35" s="13">
-        <v>1750</v>
-      </c>
+      <c r="A35" s="17"/>
+      <c r="B35" s="15"/>
+      <c r="C35" s="15"/>
+      <c r="D35" s="13"/>
       <c r="E35" s="14"/>
       <c r="F35" s="9">
         <f t="shared" si="0"/>
-        <v>34286</v>
+        <v>47286</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="14.25" customHeight="1">
@@ -1468,7 +1429,7 @@
       <c r="E36" s="14"/>
       <c r="F36" s="9">
         <f t="shared" si="0"/>
-        <v>34286</v>
+        <v>47286</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="14.25" customHeight="1">
@@ -1479,7 +1440,7 @@
       <c r="E37" s="14"/>
       <c r="F37" s="9">
         <f t="shared" si="0"/>
-        <v>34286</v>
+        <v>47286</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="14.25" customHeight="1">
@@ -1490,7 +1451,7 @@
       <c r="E38" s="14"/>
       <c r="F38" s="9">
         <f t="shared" si="0"/>
-        <v>34286</v>
+        <v>47286</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="14.25" customHeight="1">
@@ -1501,7 +1462,7 @@
       <c r="E39" s="14"/>
       <c r="F39" s="9">
         <f t="shared" si="0"/>
-        <v>34286</v>
+        <v>47286</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="14.25" customHeight="1">
@@ -1512,7 +1473,7 @@
       <c r="E40" s="14"/>
       <c r="F40" s="9">
         <f t="shared" si="0"/>
-        <v>34286</v>
+        <v>47286</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="14.25" customHeight="1">
@@ -1523,7 +1484,7 @@
       <c r="E41" s="14"/>
       <c r="F41" s="9">
         <f t="shared" si="0"/>
-        <v>34286</v>
+        <v>47286</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="14.25" customHeight="1">
@@ -1534,7 +1495,7 @@
       <c r="E42" s="14"/>
       <c r="F42" s="9">
         <f t="shared" si="0"/>
-        <v>34286</v>
+        <v>47286</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="14.25" customHeight="1">
@@ -1545,7 +1506,7 @@
       <c r="E43" s="14"/>
       <c r="F43" s="9">
         <f t="shared" si="0"/>
-        <v>34286</v>
+        <v>47286</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="14.25" customHeight="1">
@@ -1556,7 +1517,7 @@
       <c r="E44" s="14"/>
       <c r="F44" s="9">
         <f t="shared" si="0"/>
-        <v>34286</v>
+        <v>47286</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="14.25" customHeight="1">
@@ -1567,7 +1528,7 @@
       <c r="E45" s="14"/>
       <c r="F45" s="9">
         <f t="shared" si="0"/>
-        <v>34286</v>
+        <v>47286</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="14.25" customHeight="1">
@@ -1578,7 +1539,7 @@
       <c r="E46" s="14"/>
       <c r="F46" s="9">
         <f t="shared" si="0"/>
-        <v>34286</v>
+        <v>47286</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="14.25" customHeight="1">
@@ -1589,7 +1550,7 @@
       <c r="E47" s="14"/>
       <c r="F47" s="9">
         <f t="shared" si="0"/>
-        <v>34286</v>
+        <v>47286</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="14.25" customHeight="1">
@@ -1600,7 +1561,7 @@
       <c r="E48" s="14"/>
       <c r="F48" s="9">
         <f t="shared" si="0"/>
-        <v>34286</v>
+        <v>47286</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="14.25" customHeight="1">
@@ -1611,7 +1572,7 @@
       <c r="E49" s="14"/>
       <c r="F49" s="9">
         <f t="shared" si="0"/>
-        <v>34286</v>
+        <v>47286</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="14.25" customHeight="1">
@@ -1622,7 +1583,7 @@
       <c r="E50" s="14"/>
       <c r="F50" s="9">
         <f t="shared" si="0"/>
-        <v>34286</v>
+        <v>47286</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="14.25" customHeight="1">
@@ -1633,7 +1594,7 @@
       <c r="E51" s="14"/>
       <c r="F51" s="9">
         <f t="shared" si="0"/>
-        <v>34286</v>
+        <v>47286</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="14.25" customHeight="1">
@@ -1644,7 +1605,7 @@
       <c r="E52" s="14"/>
       <c r="F52" s="9">
         <f t="shared" si="0"/>
-        <v>34286</v>
+        <v>47286</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="14.25" customHeight="1">
@@ -1655,7 +1616,7 @@
       <c r="E53" s="14"/>
       <c r="F53" s="9">
         <f t="shared" si="0"/>
-        <v>34286</v>
+        <v>47286</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="14.25" customHeight="1">
@@ -1666,7 +1627,7 @@
       <c r="E54" s="14"/>
       <c r="F54" s="9">
         <f t="shared" si="0"/>
-        <v>34286</v>
+        <v>47286</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="14.25" customHeight="1">
@@ -1677,7 +1638,7 @@
       <c r="E55" s="14"/>
       <c r="F55" s="9">
         <f t="shared" si="0"/>
-        <v>34286</v>
+        <v>47286</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="14.25" customHeight="1">
@@ -1688,7 +1649,7 @@
       <c r="E56" s="14"/>
       <c r="F56" s="9">
         <f t="shared" si="0"/>
-        <v>34286</v>
+        <v>47286</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="14.25" customHeight="1">
@@ -1699,7 +1660,7 @@
       <c r="E57" s="14"/>
       <c r="F57" s="9">
         <f t="shared" si="0"/>
-        <v>34286</v>
+        <v>47286</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="14.25" customHeight="1">
@@ -1710,7 +1671,7 @@
       <c r="E58" s="14"/>
       <c r="F58" s="9">
         <f t="shared" si="0"/>
-        <v>34286</v>
+        <v>47286</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="14.25" customHeight="1">
@@ -1721,7 +1682,7 @@
       <c r="E59" s="14"/>
       <c r="F59" s="9">
         <f t="shared" si="0"/>
-        <v>34286</v>
+        <v>47286</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="14.25" customHeight="1">
@@ -1732,7 +1693,7 @@
       <c r="E60" s="14"/>
       <c r="F60" s="9">
         <f t="shared" si="0"/>
-        <v>34286</v>
+        <v>47286</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="14.25" customHeight="1">
@@ -1743,7 +1704,7 @@
       <c r="E61" s="14"/>
       <c r="F61" s="9">
         <f t="shared" si="0"/>
-        <v>34286</v>
+        <v>47286</v>
       </c>
     </row>
     <row r="62" spans="1:6" ht="14.25" customHeight="1">
@@ -1754,7 +1715,7 @@
       <c r="E62" s="14"/>
       <c r="F62" s="9">
         <f t="shared" si="0"/>
-        <v>34286</v>
+        <v>47286</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="14.25" customHeight="1">
@@ -1765,7 +1726,7 @@
       <c r="E63" s="14"/>
       <c r="F63" s="9">
         <f t="shared" si="0"/>
-        <v>34286</v>
+        <v>47286</v>
       </c>
     </row>
     <row r="64" spans="1:6" ht="14.25" customHeight="1">
@@ -1776,7 +1737,7 @@
       <c r="E64" s="14"/>
       <c r="F64" s="9">
         <f t="shared" si="0"/>
-        <v>34286</v>
+        <v>47286</v>
       </c>
     </row>
     <row r="65" spans="1:6" ht="14.25" customHeight="1">
@@ -1787,7 +1748,7 @@
       <c r="E65" s="14"/>
       <c r="F65" s="9">
         <f t="shared" si="0"/>
-        <v>34286</v>
+        <v>47286</v>
       </c>
     </row>
     <row r="66" spans="1:6" ht="14.25" customHeight="1">
@@ -1798,7 +1759,7 @@
       <c r="E66" s="14"/>
       <c r="F66" s="9">
         <f t="shared" si="0"/>
-        <v>34286</v>
+        <v>47286</v>
       </c>
     </row>
     <row r="67" spans="1:6" ht="14.25" customHeight="1">
@@ -1809,7 +1770,7 @@
       <c r="E67" s="14"/>
       <c r="F67" s="9">
         <f t="shared" si="0"/>
-        <v>34286</v>
+        <v>47286</v>
       </c>
     </row>
     <row r="68" spans="1:6" ht="14.25" customHeight="1">
@@ -1820,7 +1781,7 @@
       <c r="E68" s="14"/>
       <c r="F68" s="9">
         <f t="shared" si="0"/>
-        <v>34286</v>
+        <v>47286</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="14.25" customHeight="1">
@@ -1831,7 +1792,7 @@
       <c r="E69" s="14"/>
       <c r="F69" s="9">
         <f t="shared" si="0"/>
-        <v>34286</v>
+        <v>47286</v>
       </c>
     </row>
     <row r="70" spans="1:6" ht="14.25" customHeight="1">
@@ -1842,7 +1803,7 @@
       <c r="E70" s="14"/>
       <c r="F70" s="9">
         <f t="shared" si="0"/>
-        <v>34286</v>
+        <v>47286</v>
       </c>
     </row>
     <row r="71" spans="1:6" ht="14.25" customHeight="1">
@@ -1853,7 +1814,7 @@
       <c r="E71" s="14"/>
       <c r="F71" s="9">
         <f t="shared" si="0"/>
-        <v>34286</v>
+        <v>47286</v>
       </c>
     </row>
     <row r="72" spans="1:6" ht="14.25" customHeight="1">
@@ -1864,7 +1825,7 @@
       <c r="E72" s="14"/>
       <c r="F72" s="9">
         <f t="shared" si="0"/>
-        <v>34286</v>
+        <v>47286</v>
       </c>
     </row>
     <row r="73" spans="1:6" ht="14.25" customHeight="1">
@@ -1875,7 +1836,7 @@
       <c r="E73" s="14"/>
       <c r="F73" s="9">
         <f t="shared" si="0"/>
-        <v>34286</v>
+        <v>47286</v>
       </c>
     </row>
     <row r="74" spans="1:6" ht="14.25" customHeight="1">
@@ -1886,7 +1847,7 @@
       <c r="E74" s="14"/>
       <c r="F74" s="9">
         <f t="shared" si="0"/>
-        <v>34286</v>
+        <v>47286</v>
       </c>
     </row>
     <row r="75" spans="1:6" ht="14.25" customHeight="1">
@@ -1897,7 +1858,7 @@
       <c r="E75" s="14"/>
       <c r="F75" s="9">
         <f t="shared" si="0"/>
-        <v>34286</v>
+        <v>47286</v>
       </c>
     </row>
     <row r="76" spans="1:6" ht="14.25" customHeight="1">
@@ -1908,7 +1869,7 @@
       <c r="E76" s="14"/>
       <c r="F76" s="9">
         <f t="shared" si="0"/>
-        <v>34286</v>
+        <v>47286</v>
       </c>
     </row>
     <row r="77" spans="1:6" ht="14.25" customHeight="1">
@@ -1919,7 +1880,7 @@
       <c r="E77" s="14"/>
       <c r="F77" s="9">
         <f t="shared" si="0"/>
-        <v>34286</v>
+        <v>47286</v>
       </c>
     </row>
     <row r="78" spans="1:6" ht="14.25" customHeight="1">
@@ -1930,7 +1891,7 @@
       <c r="E78" s="14"/>
       <c r="F78" s="9">
         <f t="shared" si="0"/>
-        <v>34286</v>
+        <v>47286</v>
       </c>
     </row>
     <row r="79" spans="1:6" ht="14.25" customHeight="1">
@@ -1941,7 +1902,7 @@
       <c r="E79" s="14"/>
       <c r="F79" s="9">
         <f t="shared" si="0"/>
-        <v>34286</v>
+        <v>47286</v>
       </c>
     </row>
     <row r="80" spans="1:6" ht="14.25" customHeight="1">
@@ -1952,7 +1913,7 @@
       <c r="E80" s="14"/>
       <c r="F80" s="9">
         <f t="shared" si="0"/>
-        <v>34286</v>
+        <v>47286</v>
       </c>
     </row>
     <row r="81" spans="1:6" ht="14.25" customHeight="1">
@@ -1963,7 +1924,7 @@
       <c r="E81" s="14"/>
       <c r="F81" s="9">
         <f t="shared" si="0"/>
-        <v>34286</v>
+        <v>47286</v>
       </c>
     </row>
     <row r="82" spans="1:6" ht="14.25" customHeight="1">
@@ -1974,7 +1935,7 @@
       <c r="E82" s="14"/>
       <c r="F82" s="9">
         <f t="shared" si="0"/>
-        <v>34286</v>
+        <v>47286</v>
       </c>
     </row>
     <row r="83" spans="1:6" ht="14.25" customHeight="1">
@@ -1985,7 +1946,7 @@
       <c r="E83" s="14"/>
       <c r="F83" s="9">
         <f t="shared" si="0"/>
-        <v>34286</v>
+        <v>47286</v>
       </c>
     </row>
     <row r="84" spans="1:6" ht="14.25" customHeight="1">
@@ -1996,7 +1957,7 @@
       <c r="E84" s="14"/>
       <c r="F84" s="9">
         <f t="shared" si="0"/>
-        <v>34286</v>
+        <v>47286</v>
       </c>
     </row>
     <row r="85" spans="1:6" ht="14.25" customHeight="1">
@@ -2007,7 +1968,7 @@
       <c r="E85" s="14"/>
       <c r="F85" s="9">
         <f t="shared" si="0"/>
-        <v>34286</v>
+        <v>47286</v>
       </c>
     </row>
     <row r="86" spans="1:6" ht="14.25" customHeight="1">
@@ -2018,7 +1979,7 @@
       <c r="E86" s="14"/>
       <c r="F86" s="9">
         <f t="shared" si="0"/>
-        <v>34286</v>
+        <v>47286</v>
       </c>
     </row>
     <row r="87" spans="1:6" ht="14.25" customHeight="1">
@@ -2029,7 +1990,7 @@
       <c r="E87" s="14"/>
       <c r="F87" s="9">
         <f t="shared" si="0"/>
-        <v>34286</v>
+        <v>47286</v>
       </c>
     </row>
     <row r="88" spans="1:6" ht="14.25" customHeight="1">
@@ -2039,7 +2000,7 @@
       <c r="E88" s="14"/>
       <c r="F88" s="9">
         <f t="shared" si="0"/>
-        <v>34286</v>
+        <v>47286</v>
       </c>
     </row>
     <row r="89" spans="1:6" ht="14.25" customHeight="1">
@@ -2050,7 +2011,7 @@
       <c r="E89" s="14"/>
       <c r="F89" s="9">
         <f t="shared" si="0"/>
-        <v>34286</v>
+        <v>47286</v>
       </c>
     </row>
     <row r="90" spans="1:6" ht="14.25" customHeight="1">
@@ -2061,7 +2022,7 @@
       <c r="E90" s="14"/>
       <c r="F90" s="9">
         <f t="shared" si="0"/>
-        <v>34286</v>
+        <v>47286</v>
       </c>
     </row>
     <row r="91" spans="1:6" ht="14.25" customHeight="1">
@@ -2072,7 +2033,7 @@
       <c r="E91" s="14"/>
       <c r="F91" s="9">
         <f t="shared" si="0"/>
-        <v>34286</v>
+        <v>47286</v>
       </c>
     </row>
     <row r="92" spans="1:6" ht="14.25" customHeight="1">
@@ -2083,7 +2044,7 @@
       <c r="E92" s="14"/>
       <c r="F92" s="9">
         <f t="shared" si="0"/>
-        <v>34286</v>
+        <v>47286</v>
       </c>
     </row>
     <row r="93" spans="1:6" ht="14.25" customHeight="1">
@@ -2094,12 +2055,12 @@
       <c r="C93" s="28"/>
       <c r="D93" s="6">
         <f>SUM(D3:D92)</f>
-        <v>215714</v>
+        <v>202714</v>
       </c>
       <c r="E93" s="20"/>
       <c r="F93" s="9">
         <f t="shared" ref="F93:F94" si="1">F91</f>
-        <v>34286</v>
+        <v>47286</v>
       </c>
     </row>
     <row r="94" spans="1:6" ht="14.25" customHeight="1">
@@ -2115,7 +2076,7 @@
       </c>
       <c r="F94" s="9">
         <f t="shared" si="1"/>
-        <v>34286</v>
+        <v>47286</v>
       </c>
     </row>
     <row r="95" spans="1:6" ht="14.25" customHeight="1">
@@ -2128,7 +2089,7 @@
       <c r="E95" s="35"/>
       <c r="F95" s="22">
         <f>F92</f>
-        <v>34286</v>
+        <v>47286</v>
       </c>
     </row>
     <row r="96" spans="1:6" ht="14.25" customHeight="1"/>

</xml_diff>